<commit_message>
Update in SRS documents
</commit_message>
<xml_diff>
--- a/Technical_Documentation/Requirements/System requirement specification/UD-SRS-traceability.xlsx
+++ b/Technical_Documentation/Requirements/System requirement specification/UD-SRS-traceability.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amaliekoch/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amaliekoch/Documents/GitHub/ST6/Technical_Documentation/Requirements/System requirement specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB50D2D-4278-E64A-8118-A52B1A462900}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6BCF43-A188-F444-A86F-ADAE39513C0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28420" windowHeight="15800" xr2:uid="{B54773BD-5F2B-AF4D-8A1D-6E44CC84DFDA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
   <si>
     <t xml:space="preserve">SRS ID </t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>UD-SRS-14</t>
-  </si>
-  <si>
-    <t>UD-SRS-15</t>
   </si>
   <si>
     <t xml:space="preserve">The interface shall recommend and visualize at least three treatment strategies for the specialist </t>
@@ -164,9 +161,6 @@
     <t xml:space="preserve">UD-CRS-06 </t>
   </si>
   <si>
-    <t xml:space="preserve">The output of the system shall be graphically represented </t>
-  </si>
-  <si>
     <t>UD-SRS-16</t>
   </si>
   <si>
@@ -198,10 +192,6 @@
   </si>
   <si>
     <t>UD-CRS-07</t>
-  </si>
-  <si>
-    <t>UD-CRS-06 
-UD-CRS-07</t>
   </si>
   <si>
     <t xml:space="preserve">Ucon Sheet </t>
@@ -256,6 +246,11 @@
   </si>
   <si>
     <t xml:space="preserve">User interface "Estimate effectiveness score" shall contain information about stimulation paradigm, parameters and effectiveness score to give the specialist the opportunity to get a quick overview. </t>
+  </si>
+  <si>
+    <t>UD-CRS-03
+UD-CRS-06
+UD-CRS-07</t>
   </si>
 </sst>
 </file>
@@ -767,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865C1865-B44B-7648-9539-419D8238798C}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -789,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>3</v>
@@ -803,10 +798,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
@@ -817,10 +812,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
@@ -831,10 +826,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
@@ -845,10 +840,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -859,13 +854,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -875,10 +870,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -889,24 +884,24 @@
         <v>11</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -917,10 +912,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -931,10 +926,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -945,10 +940,10 @@
         <v>15</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -959,10 +954,10 @@
         <v>16</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -973,13 +968,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D14" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -989,38 +984,32 @@
         <v>18</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>54</v>
-      </c>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -1028,13 +1017,13 @@
     </row>
     <row r="18" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -1042,45 +1031,45 @@
     </row>
     <row r="19" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>66</v>
-      </c>
       <c r="D20" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="14"/>
@@ -1088,13 +1077,13 @@
     </row>
     <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="14"/>
@@ -1102,13 +1091,13 @@
     </row>
     <row r="23" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
@@ -1116,14 +1105,14 @@
     </row>
     <row r="24" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>

</xml_diff>